<commit_message>
update prestador hpd name v0.2.22
</commit_message>
<xml_diff>
--- a/fhir/ig/hpd/StructureDefinition-MINSALPrestadorAdministrativo.xlsx
+++ b/fhir/ig/hpd/StructureDefinition-MINSALPrestadorAdministrativo.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.1</t>
+    <t>0.2.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -13761,10 +13761,10 @@
       </c>
       <c r="E96" s="2"/>
       <c r="F96" t="s" s="2">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="G96" t="s" s="2">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="H96" t="s" s="2">
         <v>90</v>

</xml_diff>